<commit_message>
Prepare 2nd teste 2021_22
</commit_message>
<xml_diff>
--- a/exercisesLifeContingencies/lifeInsurance/makeham_wli.xlsx
+++ b/exercisesLifeContingencies/lifeInsurance/makeham_wli.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B131"/>
+  <dimension ref="A1:C131"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -447,6 +447,11 @@
           <t>Ax</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Ax_</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -455,6 +460,9 @@
       <c r="B2" t="n">
         <v>0.02131339257431903</v>
       </c>
+      <c r="C2" t="n">
+        <v>0.02183846773339848</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -463,6 +471,9 @@
       <c r="B3" t="n">
         <v>0.02216116127381717</v>
       </c>
+      <c r="C3" t="n">
+        <v>0.02270708734910754</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -471,6 +482,9 @@
       <c r="B4" t="n">
         <v>0.02305116984797573</v>
       </c>
+      <c r="C4" t="n">
+        <v>0.02361898583241229</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -479,6 +493,9 @@
       <c r="B5" t="n">
         <v>0.02398549785717418</v>
       </c>
+      <c r="C5" t="n">
+        <v>0.02457629390816973</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -487,6 +504,9 @@
       <c r="B6" t="n">
         <v>0.02496632418118079</v>
       </c>
+      <c r="C6" t="n">
+        <v>0.02558124406583362</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -495,6 +515,9 @@
       <c r="B7" t="n">
         <v>0.02599593138746477</v>
       </c>
+      <c r="C7" t="n">
+        <v>0.02663617503552584</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -503,6 +526,9 @@
       <c r="B8" t="n">
         <v>0.02707671024495758</v>
       </c>
+      <c r="C8" t="n">
+        <v>0.02774353641314986</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -511,6 +537,9 @@
       <c r="B9" t="n">
         <v>0.02821116438192677</v>
       </c>
+      <c r="C9" t="n">
+        <v>0.02890589343322503</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -519,6 +548,9 @@
       <c r="B10" t="n">
         <v>0.02940191508558346</v>
       </c>
+      <c r="C10" t="n">
+        <v>0.03012593188700063</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -527,6 +559,9 @@
       <c r="B11" t="n">
         <v>0.03065170623984182</v>
       </c>
+      <c r="C11" t="n">
+        <v>0.03140646318216045</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -535,6 +570,9 @@
       <c r="B12" t="n">
         <v>0.03196340939627151</v>
       </c>
+      <c r="C12" t="n">
+        <v>0.0327504295390646</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -543,6 +581,9 @@
       <c r="B13" t="n">
         <v>0.03334002897171479</v>
       </c>
+      <c r="C13" t="n">
+        <v>0.0341609093168419</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -551,6 +592,9 @@
       <c r="B14" t="n">
         <v>0.03478470756425205</v>
       </c>
+      <c r="C14" t="n">
+        <v>0.03564112246082207</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -559,6 +603,9 @@
       <c r="B15" t="n">
         <v>0.03630073137717097</v>
       </c>
+      <c r="C15" t="n">
+        <v>0.03719443606072736</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -567,6 +614,9 @@
       <c r="B16" t="n">
         <v>0.03789153573830823</v>
       </c>
+      <c r="C16" t="n">
+        <v>0.03882437000666317</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -575,6 +625,9 @@
       <c r="B17" t="n">
         <v>0.03956071069954484</v>
       </c>
+      <c r="C17" t="n">
+        <v>0.04053460272736675</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -583,6 +636,9 @@
       <c r="B18" t="n">
         <v>0.04131200669833626</v>
       </c>
+      <c r="C18" t="n">
+        <v>0.04232897699213733</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -591,6 +647,9 @@
       <c r="B19" t="n">
         <v>0.0431493402599024</v>
       </c>
+      <c r="C19" t="n">
+        <v>0.04421150575457011</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -599,6 +658,9 @@
       <c r="B20" t="n">
         <v>0.04507679971506211</v>
       </c>
+      <c r="C20" t="n">
+        <v>0.04618637801248482</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -607,6 +669,9 @@
       <c r="B21" t="n">
         <v>0.04709865090463529</v>
       </c>
+      <c r="C21" t="n">
+        <v>0.0482579646542689</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -615,6 +680,9 @@
       <c r="B22" t="n">
         <v>0.04921934283681906</v>
       </c>
+      <c r="C22" t="n">
+        <v>0.05043082425724899</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -623,6 +691,9 @@
       <c r="B23" t="n">
         <v>0.05144351325892879</v>
       </c>
+      <c r="C23" t="n">
+        <v>0.05270970879854797</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -631,6 +702,9 @@
       <c r="B24" t="n">
         <v>0.05377599409934607</v>
       </c>
+      <c r="C24" t="n">
+        <v>0.05509956923321591</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -639,6 +713,9 @@
       <c r="B25" t="n">
         <v>0.05622181672938697</v>
       </c>
+      <c r="C25" t="n">
+        <v>0.05760556088814617</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -647,6 +724,9 @@
       <c r="B26" t="n">
         <v>0.05878621698805893</v>
       </c>
+      <c r="C26" t="n">
+        <v>0.06023304861331924</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -655,6 +735,9 @@
       <c r="B27" t="n">
         <v>0.06147463990526979</v>
       </c>
+      <c r="C27" t="n">
+        <v>0.0629876116247734</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -663,6 +746,9 @@
       <c r="B28" t="n">
         <v>0.06429274405094447</v>
       </c>
+      <c r="C28" t="n">
+        <v>0.06587504796388388</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -671,6 +757,9 @@
       <c r="B29" t="n">
         <v>0.06724640542866429</v>
       </c>
+      <c r="C29" t="n">
+        <v>0.06890137849155775</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -679,6 +768,9 @@
       <c r="B30" t="n">
         <v>0.07034172082282271</v>
       </c>
+      <c r="C30" t="n">
+        <v>0.07207285032207433</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -687,6 +779,9 @@
       <c r="B31" t="n">
         <v>0.07358501049787318</v>
       </c>
+      <c r="C31" t="n">
+        <v>0.07539593959417823</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -695,6 +790,9 @@
       <c r="B32" t="n">
         <v>0.07698282013699637</v>
       </c>
+      <c r="C32" t="n">
+        <v>0.07887735346338687</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -703,6 +801,9 @@
       <c r="B33" t="n">
         <v>0.08054192189542504</v>
       </c>
+      <c r="C33" t="n">
+        <v>0.08252403118791796</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -711,6 +812,9 @@
       <c r="B34" t="n">
         <v>0.08426931443073285</v>
       </c>
+      <c r="C34" t="n">
+        <v>0.08634314488640094</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -719,6 +823,9 @@
       <c r="B35" t="n">
         <v>0.08817222175862861</v>
       </c>
+      <c r="C35" t="n">
+        <v>0.09034209477851418</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -727,6 +834,9 @@
       <c r="B36" t="n">
         <v>0.09225809076823245</v>
       </c>
+      <c r="C36" t="n">
+        <v>0.09452851383970862</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -735,6 +845,9 @@
       <c r="B37" t="n">
         <v>0.09653458721549465</v>
       </c>
+      <c r="C37" t="n">
+        <v>0.0989102565158152</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -743,6 +856,9 @@
       <c r="B38" t="n">
         <v>0.1010095899974369</v>
       </c>
+      <c r="C38" t="n">
+        <v>0.1034953964640188</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -751,6 +867,9 @@
       <c r="B39" t="n">
         <v>0.1056911834933572</v>
       </c>
+      <c r="C39" t="n">
+        <v>0.1082922180001886</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -759,6 +878,9 @@
       <c r="B40" t="n">
         <v>0.1105876477422001</v>
       </c>
+      <c r="C40" t="n">
+        <v>0.1133092060498886</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -767,6 +889,9 @@
       <c r="B41" t="n">
         <v>0.1157074462081464</v>
       </c>
+      <c r="C41" t="n">
+        <v>0.1185550336302262</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -775,6 +900,9 @@
       <c r="B42" t="n">
         <v>0.1210592108693797</v>
       </c>
+      <c r="C42" t="n">
+        <v>0.1240385465911286</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -783,6 +911,9 @@
       <c r="B43" t="n">
         <v>0.1266517243482454</v>
       </c>
+      <c r="C43" t="n">
+        <v>0.1297687453276781</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -791,6 +922,9 @@
       <c r="B44" t="n">
         <v>0.1324938987850207</v>
       </c>
+      <c r="C44" t="n">
+        <v>0.1357547631586213</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -799,6 +933,9 @@
       <c r="B45" t="n">
         <v>0.1385947511427214</v>
       </c>
+      <c r="C45" t="n">
+        <v>0.1420058410511875</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -807,6 +944,9 @@
       <c r="B46" t="n">
         <v>0.1449633746173355</v>
       </c>
+      <c r="C46" t="n">
+        <v>0.1485312983589038</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -815,6 +955,9 @@
       <c r="B47" t="n">
         <v>0.1516089058172471</v>
       </c>
+      <c r="C47" t="n">
+        <v>0.1553404992284082</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -823,6 +966,9 @@
       <c r="B48" t="n">
         <v>0.158540487368153</v>
       </c>
+      <c r="C48" t="n">
+        <v>0.1624428143234935</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -831,6 +977,9 @@
       <c r="B49" t="n">
         <v>0.1657672255963593</v>
       </c>
+      <c r="C49" t="n">
+        <v>0.1698475775113208</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -839,6 +988,9 @@
       <c r="B50" t="n">
         <v>0.1732981429449653</v>
       </c>
+      <c r="C50" t="n">
+        <v>0.1775640371574115</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -847,6 +999,9 @@
       <c r="B51" t="n">
         <v>0.1811421247852415</v>
       </c>
+      <c r="C51" t="n">
+        <v>0.1856013016840466</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -855,6 +1010,9 @@
       <c r="B52" t="n">
         <v>0.1893078603007285</v>
       </c>
+      <c r="C52" t="n">
+        <v>0.1939682790650441</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -863,6 +1021,9 @@
       <c r="B53" t="n">
         <v>0.197803777145623</v>
       </c>
+      <c r="C53" t="n">
+        <v>0.2026736099329353</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -871,6 +1032,9 @@
       <c r="B54" t="n">
         <v>0.2066379696133816</v>
       </c>
+      <c r="C54" t="n">
+        <v>0.2117255940893398</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -879,6 +1043,9 @@
       <c r="B55" t="n">
         <v>0.2158181200977749</v>
       </c>
+      <c r="C55" t="n">
+        <v>0.2211321100897944</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -887,6 +1054,9 @@
       <c r="B56" t="n">
         <v>0.2253514136885641</v>
       </c>
+      <c r="C56" t="n">
+        <v>0.2309005278552871</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -895,6 +1065,9 @@
       <c r="B57" t="n">
         <v>0.2352444458192947</v>
       </c>
+      <c r="C57" t="n">
+        <v>0.2410376141570991</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -903,6 +1076,9 @@
       <c r="B58" t="n">
         <v>0.2455031229771621</v>
       </c>
+      <c r="C58" t="n">
+        <v>0.2515494310090365</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -911,6 +1087,9 @@
       <c r="B59" t="n">
         <v>0.2561325565961908</v>
       </c>
+      <c r="C59" t="n">
+        <v>0.2624412270915558</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -919,6 +1098,9 @@
       <c r="B60" t="n">
         <v>0.2671369503866425</v>
       </c>
+      <c r="C60" t="n">
+        <v>0.2737173224681603</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -927,6 +1109,9 @@
       <c r="B61" t="n">
         <v>0.2785194815069554</v>
       </c>
+      <c r="C61" t="n">
+        <v>0.2853809870123595</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -935,6 +1120,9 @@
       <c r="B62" t="n">
         <v>0.290282176160605</v>
       </c>
+      <c r="C62" t="n">
+        <v>0.2974343131445313</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -943,6 +1131,9 @@
       <c r="B63" t="n">
         <v>0.3024257803995438</v>
       </c>
+      <c r="C63" t="n">
+        <v>0.3098780836821342</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -951,6 +1142,9 @@
       <c r="B64" t="n">
         <v>0.3149496271382108</v>
       </c>
+      <c r="C64" t="n">
+        <v>0.3227116358351644</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -959,6 +1153,9 @@
       <c r="B65" t="n">
         <v>0.3278515006265114</v>
       </c>
+      <c r="C65" t="n">
+        <v>0.3359327226292517</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -967,6 +1164,9 @@
       <c r="B66" t="n">
         <v>0.341127499894705</v>
       </c>
+      <c r="C66" t="n">
+        <v>0.3495373733106375</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -975,6 +1175,9 @@
       <c r="B67" t="n">
         <v>0.3547719029646143</v>
       </c>
+      <c r="C67" t="n">
+        <v>0.3635197545757143</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -983,6 +1186,9 @@
       <c r="B68" t="n">
         <v>0.3687770339153911</v>
       </c>
+      <c r="C68" t="n">
+        <v>0.3778720347697695</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -991,6 +1197,9 @@
       <c r="B69" t="n">
         <v>0.3831331351920205</v>
       </c>
+      <c r="C69" t="n">
+        <v>0.3925842535072673</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -999,6 +1208,9 @@
       <c r="B70" t="n">
         <v>0.3978282478428288</v>
       </c>
+      <c r="C70" t="n">
+        <v>0.4076441994722695</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -1007,6 +1219,9 @@
       <c r="B71" t="n">
         <v>0.4128481026585593</v>
       </c>
+      <c r="C71" t="n">
+        <v>0.4230372994515147</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
@@ -1015,6 +1230,9 @@
       <c r="B72" t="n">
         <v>0.4281760254481776</v>
       </c>
+      <c r="C72" t="n">
+        <v>0.4387465219228787</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
@@ -1023,6 +1241,9 @@
       <c r="B73" t="n">
         <v>0.4437928599116089</v>
       </c>
+      <c r="C73" t="n">
+        <v>0.454752298753054</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
@@ -1031,6 +1252,9 @@
       <c r="B74" t="n">
         <v>0.4596769117413889</v>
       </c>
+      <c r="C74" t="n">
+        <v>0.4710324687358843</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -1039,6 +1263,9 @@
       <c r="B75" t="n">
         <v>0.4758039176864697</v>
       </c>
+      <c r="C75" t="n">
+        <v>0.4875622468073545</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -1047,6 +1274,9 @@
       <c r="B76" t="n">
         <v>0.4921470433238678</v>
       </c>
+      <c r="C76" t="n">
+        <v>0.5043142227875714</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -1055,6 +1285,9 @@
       <c r="B77" t="n">
         <v>0.5086769131886827</v>
       </c>
+      <c r="C77" t="n">
+        <v>0.5212583934040509</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -1063,6 +1296,9 @@
       <c r="B78" t="n">
         <v>0.525361676691967</v>
       </c>
+      <c r="C78" t="n">
+        <v>0.538362231125875</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
@@ -1071,6 +1307,9 @@
       <c r="B79" t="n">
         <v>0.5421671128922168</v>
       </c>
+      <c r="C79" t="n">
+        <v>0.5555907929675706</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
@@ -1079,6 +1318,9 @@
       <c r="B80" t="n">
         <v>0.5590567766659129</v>
       </c>
+      <c r="C80" t="n">
+        <v>0.5729068718905337</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -1087,6 +1329,9 @@
       <c r="B81" t="n">
         <v>0.5759921881359816</v>
       </c>
+      <c r="C81" t="n">
+        <v>0.5902711927289979</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
@@ -1095,6 +1340,9 @@
       <c r="B82" t="n">
         <v>0.592933066360474</v>
       </c>
+      <c r="C82" t="n">
+        <v>0.6076426536922175</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
@@ -1103,6 +1351,9 @@
       <c r="B83" t="n">
         <v>0.6098376072609744</v>
       </c>
+      <c r="C83" t="n">
+        <v>0.6249786134500703</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -1111,6 +1362,9 @@
       <c r="B84" t="n">
         <v>0.6266628045939696</v>
       </c>
+      <c r="C84" t="n">
+        <v>0.6422352226071124</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -1119,6 +1373,9 @@
       <c r="B85" t="n">
         <v>0.6433648114617025</v>
       </c>
+      <c r="C85" t="n">
+        <v>0.6593677970349821</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -1127,6 +1384,9 @@
       <c r="B86" t="n">
         <v>0.6598993384560086</v>
       </c>
+      <c r="C86" t="n">
+        <v>0.6763312290997248</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -1135,6 +1395,9 @@
       <c r="B87" t="n">
         <v>0.6762220830748427</v>
       </c>
+      <c r="C87" t="n">
+        <v>0.6930804313355352</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
@@ -1143,6 +1406,9 @@
       <c r="B88" t="n">
         <v>0.692289183602941</v>
       </c>
+      <c r="C88" t="n">
+        <v>0.7095708056367056</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -1151,6 +1417,9 @@
       <c r="B89" t="n">
         <v>0.7080576892710713</v>
       </c>
+      <c r="C89" t="n">
+        <v>0.725758729635308</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -1159,6 +1428,9 @@
       <c r="B90" t="n">
         <v>0.7234860372751407</v>
       </c>
+      <c r="C90" t="n">
+        <v>0.7416020506721074</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -1167,6 +1439,9 @@
       <c r="B91" t="n">
         <v>0.7385345262230144</v>
       </c>
+      <c r="C91" t="n">
+        <v>0.7570605767369721</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -1175,6 +1450,9 @@
       <c r="B92" t="n">
         <v>0.7531657748579331</v>
       </c>
+      <c r="C92" t="n">
+        <v>0.7720965530230101</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
@@ -1183,6 +1461,9 @@
       <c r="B93" t="n">
         <v>0.7673451545512801</v>
       </c>
+      <c r="C93" t="n">
+        <v>0.7866751123789689</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
@@ -1191,6 +1472,9 @@
       <c r="B94" t="n">
         <v>0.7810411841203093</v>
       </c>
+      <c r="C94" t="n">
+        <v>0.8007646880128469</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
@@ -1199,6 +1483,9 @@
       <c r="B95" t="n">
         <v>0.7942258760468284</v>
       </c>
+      <c r="C95" t="n">
+        <v>0.8143373773350518</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
@@ -1207,6 +1494,9 @@
       <c r="B96" t="n">
         <v>0.8068750241664815</v>
       </c>
+      <c r="C96" t="n">
+        <v>0.827369246846828</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
@@ -1215,6 +1505,9 @@
       <c r="B97" t="n">
         <v>0.8189684243544572</v>
       </c>
+      <c r="C97" t="n">
+        <v>0.8398405694662308</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
@@ -1223,6 +1516,9 @@
       <c r="B98" t="n">
         <v>0.8304900216129066</v>
       </c>
+      <c r="C98" t="n">
+        <v>0.8517359875969845</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
@@ -1231,6 +1527,9 @@
       <c r="B99" t="n">
         <v>0.841427979200783</v>
       </c>
+      <c r="C99" t="n">
+        <v>0.8630445975125538</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
@@ -1239,6 +1538,9 @@
       <c r="B100" t="n">
         <v>0.8517746679457944</v>
       </c>
+      <c r="C100" t="n">
+        <v>0.8737599531487861</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
@@ -1247,6 +1549,9 @@
       <c r="B101" t="n">
         <v>0.8615265765290623</v>
       </c>
+      <c r="C101" t="n">
+        <v>0.8838799900519639</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
@@ -1255,6 +1560,9 @@
       <c r="B102" t="n">
         <v>0.8706841462132785</v>
       </c>
+      <c r="C102" t="n">
+        <v>0.8934068728791764</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
@@ -1263,6 +1571,9 @@
       <c r="B103" t="n">
         <v>0.8792515360716443</v>
       </c>
+      <c r="C103" t="n">
+        <v>0.9023467723543033</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
@@ -1271,6 +1582,9 @@
       <c r="B104" t="n">
         <v>0.8872363271555272</v>
       </c>
+      <c r="C104" t="n">
+        <v>0.9107095798114119</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
@@ -1279,6 +1593,9 @@
       <c r="B105" t="n">
         <v>0.8946491761245994</v>
       </c>
+      <c r="C105" t="n">
+        <v>0.9185085692903686</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
@@ -1287,6 +1604,9 @@
       <c r="B106" t="n">
         <v>0.9015034305985862</v>
       </c>
+      <c r="C106" t="n">
+        <v>0.9257600184956263</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -1295,6 +1615,9 @@
       <c r="B107" t="n">
         <v>0.9078147198611326</v>
       </c>
+      <c r="C107" t="n">
+        <v>0.9324828007298374</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -1303,6 +1626,9 @@
       <c r="B108" t="n">
         <v>0.9136005355860272</v>
       </c>
+      <c r="C108" t="n">
+        <v>0.9386979601485927</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -1311,6 +1637,9 @@
       <c r="B109" t="n">
         <v>0.9188798180405563</v>
       </c>
+      <c r="C109" t="n">
+        <v>0.9444282823679473</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -1319,6 +1648,9 @@
       <c r="B110" t="n">
         <v>0.9236725638590978</v>
       </c>
+      <c r="C110" t="n">
+        <v>0.9496978716448743</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -1327,6 +1659,9 @@
       <c r="B111" t="n">
         <v>0.9279994720883868</v>
       </c>
+      <c r="C111" t="n">
+        <v>0.9545317446237099</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -1335,6 +1670,9 @@
       <c r="B112" t="n">
         <v>0.9318816458603624</v>
       </c>
+      <c r="C112" t="n">
+        <v>0.958955449101193</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -1343,6 +1681,9 @@
       <c r="B113" t="n">
         <v>0.9353403677055223</v>
       </c>
+      <c r="C113" t="n">
+        <v>0.9629947145221771</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -1351,6 +1692,9 @@
       <c r="B114" t="n">
         <v>0.9383969668908788</v>
       </c>
+      <c r="C114" t="n">
+        <v>0.9666751390920042</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -1359,6 +1703,9 @@
       <c r="B115" t="n">
         <v>0.9410727965391654</v>
       </c>
+      <c r="C115" t="n">
+        <v>0.9700219165866659</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -1367,6 +1714,9 @@
       <c r="B116" t="n">
         <v>0.9433893353033589</v>
       </c>
+      <c r="C116" t="n">
+        <v>0.973059604249833</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
@@ -1375,6 +1725,9 @@
       <c r="B117" t="n">
         <v>0.9453684208453996</v>
       </c>
+      <c r="C117" t="n">
+        <v>0.9758119316584863</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -1383,6 +1736,9 @@
       <c r="B118" t="n">
         <v>0.9470326073258055</v>
       </c>
+      <c r="C118" t="n">
+        <v>0.9783016491651689</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -1391,6 +1747,9 @@
       <c r="B119" t="n">
         <v>0.948405613452685</v>
       </c>
+      <c r="C119" t="n">
+        <v>0.9805504135116315</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
@@ -1399,6 +1758,9 @@
       <c r="B120" t="n">
         <v>0.9495127899841558</v>
       </c>
+      <c r="C120" t="n">
+        <v>0.9825787074617135</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
@@ -1407,6 +1769,9 @@
       <c r="B121" t="n">
         <v>0.9503814896985835</v>
       </c>
+      <c r="C121" t="n">
+        <v>0.9844057898093281</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
@@ -1415,6 +1780,9 @@
       <c r="B122" t="n">
         <v>0.9510411820338167</v>
       </c>
+      <c r="C122" t="n">
+        <v>0.9860496718562833</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
@@ -1423,6 +1791,9 @@
       <c r="B123" t="n">
         <v>0.9515231438742534</v>
       </c>
+      <c r="C123" t="n">
+        <v>0.9875271163905259</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
@@ -1431,6 +1802,9 @@
       <c r="B124" t="n">
         <v>0.951859608261596</v>
       </c>
+      <c r="C124" t="n">
+        <v>0.9888536552920273</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -1439,6 +1813,9 @@
       <c r="B125" t="n">
         <v>0.9520823821744701</v>
       </c>
+      <c r="C125" t="n">
+        <v>0.9900436221109798</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
@@ -1447,6 +1824,9 @@
       <c r="B126" t="n">
         <v>0.9522211315747523</v>
       </c>
+      <c r="C126" t="n">
+        <v>0.9911101962660576</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
@@ -1455,6 +1835,9 @@
       <c r="B127" t="n">
         <v>0.9523017031150203</v>
       </c>
+      <c r="C127" t="n">
+        <v>0.9920654558659634</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
@@ -1463,6 +1846,9 @@
       <c r="B128" t="n">
         <v>0.9523449085090447</v>
       </c>
+      <c r="C128" t="n">
+        <v>0.9929204365380463</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
@@ -1471,6 +1857,9 @@
       <c r="B129" t="n">
         <v>0.9523660803333406</v>
       </c>
+      <c r="C129" t="n">
+        <v>0.9936851940313892</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
@@ -1479,6 +1868,9 @@
       <c r="B130" t="n">
         <v>0.952375453391482</v>
       </c>
+      <c r="C130" t="n">
+        <v>0.9943688687318274</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
@@ -1486,6 +1878,9 @@
       </c>
       <c r="B131" t="n">
         <v>0.9523809523809523</v>
+      </c>
+      <c r="C131" t="n">
+        <v>0.9949797505712356</v>
       </c>
     </row>
   </sheetData>

</xml_diff>